<commit_message>
Mon Oct 28 09:19:51 PM EDT 2024
</commit_message>
<xml_diff>
--- a/SHAP/all_Hn_shap.xlsx
+++ b/SHAP/all_Hn_shap.xlsx
@@ -447,11 +447,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pair_energy</t>
+          <t>coulomb</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -460,11 +460,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>coulomb</t>
+          <t>occr4</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -512,11 +512,11 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>occr4</t>
+          <t>SCFOCCr4</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -564,11 +564,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SCFOCCr4</t>
+          <t>SCFFp</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -590,54 +590,54 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SCFFp</t>
+          <t>pair_energy</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>7.716963870198247e-11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SCFOCCs3</t>
+          <t>SCFOCCs4</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.440635276675457e-07</v>
+        <v>2.325172841517294e-07</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SCFOCCs4</t>
+          <t>SCFOCCs2</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.447441430595629e-07</v>
+        <v>2.342662069568913e-07</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SCFOCCs2</t>
+          <t>SCFOCCs3</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.591284456887324e-07</v>
+        <v>2.426294550217148e-07</v>
       </c>
     </row>
     <row r="17">
@@ -650,46 +650,46 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.599695897811424e-07</v>
+        <v>2.777837984205288e-07</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SCFOCCq</t>
+          <t>hqq</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.848363666382365e-07</v>
+        <v>2.884392512463198e-07</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SCFOCCp</t>
+          <t>SCFOCCq</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.881764657529938e-07</v>
+        <v>2.887254040271499e-07</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>hqq</t>
+          <t>SCFOCCp</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.014436259660197e-07</v>
+        <v>2.991790885353124e-07</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.375889446415459e-07</v>
+        <v>8.583691881192582e-07</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.053058507696927e-06</v>
+        <v>1.053489669616333e-06</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.06935724467379e-06</v>
+        <v>1.083748446022736e-06</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.963580837391767e-06</v>
+        <v>1.885888150651915e-06</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.708310443358151e-06</v>
+        <v>3.677954911480495e-06</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.08342748429842e-06</v>
+        <v>4.166896442014128e-06</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6.082043244224446e-06</v>
+        <v>6.082808949942495e-06</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6.237703553491447e-06</v>
+        <v>6.267799861822713e-06</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>7.530081742207543e-06</v>
+        <v>7.644434890804024e-06</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.691842504842444e-06</v>
+        <v>9.786079668646735e-06</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.163617319477578e-05</v>
+        <v>1.160236817893111e-05</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.25737210306376e-05</v>
+        <v>1.246321771416641e-05</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1.295952127476703e-05</v>
+        <v>1.285734420393612e-05</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.523138387953625e-05</v>
+        <v>1.533054277918431e-05</v>
       </c>
     </row>
     <row r="35">
@@ -884,46 +884,46 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.566386487639073e-05</v>
+        <v>1.534470392386801e-05</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>hss1</t>
+          <t>hss2</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.636193227510531e-05</v>
+        <v>1.67000580812405e-05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>hss2</t>
+          <t>hss1</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1.672003992862567e-05</v>
+        <v>1.689288264658724e-05</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fs3</t>
+          <t>eijab_3</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1.80107996066734e-05</v>
+        <v>1.809746288411477e-05</v>
       </c>
     </row>
     <row r="39">
@@ -936,20 +936,20 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.807973688930613e-05</v>
+        <v>1.812935385762642e-05</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>eijab_3</t>
+          <t>Fs3</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.831716704848798e-05</v>
+        <v>1.824138155036271e-05</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.897822331838242e-05</v>
+        <v>1.92359541372374e-05</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.111386289088786e-05</v>
+        <v>2.118160951747545e-05</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2.166871830593401e-05</v>
+        <v>2.167753923753714e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2.417554283962197e-05</v>
+        <v>2.393468630956089e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2.493644087235225e-05</v>
+        <v>2.479385293874846e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2.535790738745527e-05</v>
+        <v>2.534631068421036e-05</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2.736354395753088e-05</v>
+        <v>2.7245629097016e-05</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2.817625990976507e-05</v>
+        <v>2.834766055828733e-05</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.026087523177783e-05</v>
+        <v>3.04776222587208e-05</v>
       </c>
     </row>
     <row r="50">
@@ -1079,33 +1079,33 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.102042546242687e-05</v>
+        <v>3.135206226056221e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>screenvirt_4</t>
+          <t>SCFFs4</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.169386631222096e-05</v>
+        <v>3.178245358218824e-05</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SCFFs4</t>
+          <t>screenvirt_4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3.206805594713987e-05</v>
+        <v>3.207539147244977e-05</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.338931831365347e-05</v>
+        <v>3.288769948605978e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.521739456559812e-05</v>
+        <v>3.494307314350983e-05</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.534331747608286e-05</v>
+        <v>3.514199163176058e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.624475055735166e-05</v>
+        <v>3.650377376256499e-05</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3.857227010966883e-05</v>
+        <v>3.866612528759924e-05</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4.171780480771251e-05</v>
+        <v>4.151725316181081e-05</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4.267451285869306e-05</v>
+        <v>4.245195593576835e-05</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>4.513569137508376e-05</v>
+        <v>4.522295191001501e-05</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4.826797981055308e-05</v>
+        <v>4.823712106852731e-05</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>5.011002409302602e-05</v>
+        <v>4.980231149011689e-05</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>5.34791785450605e-05</v>
+        <v>5.322045189521259e-05</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>5.37114667249692e-05</v>
+        <v>5.352977670267405e-05</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.355921303167399e-05</v>
+        <v>6.351828417088331e-05</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>6.52220098076606e-05</v>
+        <v>6.541616762866939e-05</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>6.656912308810293e-05</v>
+        <v>6.593858394030188e-05</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>6.939995573429851e-05</v>
+        <v>6.915529427541604e-05</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>7.357840401504704e-05</v>
+        <v>7.398755716951347e-05</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.0001805339976879281</v>
+        <v>0.000180491434114067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>